<commit_message>
changed format to HIGH QUALITY
</commit_message>
<xml_diff>
--- a/public/titem_new.xlsx
+++ b/public/titem_new.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -483,6 +483,7 @@
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -531,11 +532,16 @@
           <t>Satuan Unit</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Nama Vendor</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="45" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Finish Good / Raw Material / Service</t>
+          <t>High Quality / Raw Material / Service</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -578,11 +584,16 @@
           <t>Satuan unit (wajib diisi, harus sudah terdaftar, contoh: pcs, kg, box)</t>
         </is>
       </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Nama Vendor (opsional, harus sudah terdaftar, contoh: Vendor A)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Finish Good</t>
+          <t>High Quality</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -619,6 +630,11 @@
           <t>pcs</t>
         </is>
       </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Vendor A</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="F4" s="5" t="n"/>
@@ -5607,7 +5623,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A3:A1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Input Tidak Valid" error="Pilih salah satu: Finish Good, Raw Material, atau Service" promptTitle="Tipe Item" prompt="Pilih tipe item dari dropdown" type="list">
+    <dataValidation sqref="A3:A1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Input Tidak Valid" error="Pilih salah satu: High Quality, Raw Material, atau Service" promptTitle="Tipe Item" prompt="Pilih tipe item dari dropdown" type="list">
       <formula1>Dropdown_Reference!$A$2:$A$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -5642,7 +5658,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Finish Good</t>
+          <t>High Quality</t>
         </is>
       </c>
     </row>

</xml_diff>